<commit_message>
using the login credentials Teacher can login in Teachers page
Signed-off-by: Samir Gorai <samirgorai17@gmail.com>
</commit_message>
<xml_diff>
--- a/input data/teacher_data.xlsx
+++ b/input data/teacher_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samir\LearnDjangoUdemy\E_Learning_folder\input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDA8C18-ED4C-42AA-8D90-A30EC903AFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF270C5-2CC0-4DB4-A3A2-DDD705243708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>teacher_first_name</t>
   </si>
@@ -64,6 +64,45 @@
   </si>
   <si>
     <t>kavita@gmail.com</t>
+  </si>
+  <si>
+    <t>Hulk</t>
+  </si>
+  <si>
+    <t>Hogan</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Hulk@gmail.com</t>
+  </si>
+  <si>
+    <t>rey</t>
+  </si>
+  <si>
+    <t>meystario</t>
+  </si>
+  <si>
+    <t>rey@gmail.com</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Gope</t>
+  </si>
+  <si>
+    <t>Ram@gmail.com</t>
+  </si>
+  <si>
+    <t>Junu</t>
+  </si>
+  <si>
+    <t>majhi</t>
+  </si>
+  <si>
+    <t>junu@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -401,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,10 +516,94 @@
         <v>3333333333</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2">
+        <v>34001</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>7777777777</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2">
+        <v>35827</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>6666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2">
+        <v>32984</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>9999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2">
+        <v>33635</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>5555555555</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{521CA714-1823-47E9-AD14-DC9851C0A911}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{29C3A51C-D1A8-4323-9EFF-9E1FAB285C9C}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{DC75D930-BD70-4789-8A80-7E6AA697FA48}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{7E7AEE62-569B-4B16-BEE8-9A9B457754B7}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{4E68AFCA-32E4-4101-86B4-A15D050D77E5}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{535BFFCB-ABF8-4208-97E6-CE9EECBDCDCE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>